<commit_message>
First per led control commit
</commit_message>
<xml_diff>
--- a/HUEAmbientProtocol.xlsx
+++ b/HUEAmbientProtocol.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\NZXTHUEAmbient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6005206B-2DDB-45DC-98E6-71CBF6477743}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6AB3D0B-C49F-4C01-B5D8-2D78C6815BBE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8ACBE584-7051-4F8D-8C1E-5A46D2609478}"/>
+    <workbookView xWindow="16635" yWindow="2610" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{8ACBE584-7051-4F8D-8C1E-5A46D2609478}"/>
   </bookViews>
   <sheets>
     <sheet name="Per led command" sheetId="1" r:id="rId1"/>
-    <sheet name="All led command" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="3" r:id="rId2"/>
+    <sheet name="All led command" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -487,7 +488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -520,27 +521,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -549,8 +532,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -576,9 +559,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -895,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CDE378C-8288-4289-8270-BA992A9299D4}">
   <dimension ref="B2:K66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView showGridLines="0" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,18 +921,18 @@
       <c r="D2" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14" t="s">
+      <c r="F2" s="26"/>
+      <c r="G2" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="I2" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="J2" s="24"/>
-      <c r="K2" s="25"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="19"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="10">
@@ -942,16 +944,16 @@
       <c r="D3" s="6">
         <v>22</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="27">
         <v>22</v>
       </c>
-      <c r="F3" s="16"/>
+      <c r="F3" s="27"/>
       <c r="G3" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="I3" s="26"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="28"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="22"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="10">
@@ -972,9 +974,9 @@
       <c r="G4" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="I4" s="26"/>
-      <c r="J4" s="27"/>
-      <c r="K4" s="28"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="22"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="10">
@@ -996,9 +998,9 @@
         <v>71</v>
       </c>
       <c r="H5" s="1"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="28"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="22"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="10">
@@ -1010,17 +1012,17 @@
       <c r="D6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6" s="17"/>
+      <c r="E6" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="28"/>
       <c r="G6" s="4" t="s">
         <v>74</v>
       </c>
       <c r="H6" s="1"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="31"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="24"/>
+      <c r="K6" s="25"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="10">
@@ -1032,10 +1034,10 @@
       <c r="D7" s="9">
         <v>255</v>
       </c>
-      <c r="E7" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="22"/>
+      <c r="E7" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="16"/>
       <c r="G7" s="4" t="s">
         <v>77</v>
       </c>
@@ -1050,10 +1052,10 @@
       <c r="D8" s="9">
         <v>255</v>
       </c>
-      <c r="E8" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="22"/>
+      <c r="E8" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="16"/>
       <c r="G8" s="4" t="s">
         <v>78</v>
       </c>
@@ -1068,10 +1070,10 @@
       <c r="D9" s="9">
         <v>255</v>
       </c>
-      <c r="E9" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="22"/>
+      <c r="E9" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="16"/>
       <c r="G9" s="4" t="s">
         <v>79</v>
       </c>
@@ -1086,10 +1088,10 @@
       <c r="D10" s="9">
         <v>255</v>
       </c>
-      <c r="E10" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" s="22"/>
+      <c r="E10" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="16"/>
       <c r="G10" s="4" t="s">
         <v>77</v>
       </c>
@@ -1104,10 +1106,10 @@
       <c r="D11" s="9">
         <v>255</v>
       </c>
-      <c r="E11" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="22"/>
+      <c r="E11" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="16"/>
       <c r="G11" s="4" t="s">
         <v>78</v>
       </c>
@@ -1122,10 +1124,10 @@
       <c r="D12" s="9">
         <v>255</v>
       </c>
-      <c r="E12" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F12" s="22"/>
+      <c r="E12" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="16"/>
       <c r="G12" s="4" t="s">
         <v>79</v>
       </c>
@@ -1140,10 +1142,10 @@
       <c r="D13" s="9">
         <v>255</v>
       </c>
-      <c r="E13" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="22"/>
+      <c r="E13" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="16"/>
       <c r="G13" s="4" t="s">
         <v>77</v>
       </c>
@@ -1158,10 +1160,10 @@
       <c r="D14" s="9">
         <v>255</v>
       </c>
-      <c r="E14" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="22"/>
+      <c r="E14" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="16"/>
       <c r="G14" s="4" t="s">
         <v>78</v>
       </c>
@@ -1176,10 +1178,10 @@
       <c r="D15" s="9">
         <v>255</v>
       </c>
-      <c r="E15" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="22"/>
+      <c r="E15" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="16"/>
       <c r="G15" s="4" t="s">
         <v>79</v>
       </c>
@@ -1194,10 +1196,10 @@
       <c r="D16" s="9">
         <v>255</v>
       </c>
-      <c r="E16" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="22"/>
+      <c r="E16" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="16"/>
       <c r="G16" s="4" t="s">
         <v>77</v>
       </c>
@@ -1212,10 +1214,10 @@
       <c r="D17" s="9">
         <v>255</v>
       </c>
-      <c r="E17" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="22"/>
+      <c r="E17" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="16"/>
       <c r="G17" s="4" t="s">
         <v>78</v>
       </c>
@@ -1230,10 +1232,10 @@
       <c r="D18" s="9">
         <v>255</v>
       </c>
-      <c r="E18" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F18" s="22"/>
+      <c r="E18" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="16"/>
       <c r="G18" s="4" t="s">
         <v>79</v>
       </c>
@@ -1248,10 +1250,10 @@
       <c r="D19" s="9">
         <v>255</v>
       </c>
-      <c r="E19" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="22"/>
+      <c r="E19" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="16"/>
       <c r="G19" s="4" t="s">
         <v>77</v>
       </c>
@@ -1266,10 +1268,10 @@
       <c r="D20" s="9">
         <v>255</v>
       </c>
-      <c r="E20" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F20" s="22"/>
+      <c r="E20" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="16"/>
       <c r="G20" s="4" t="s">
         <v>78</v>
       </c>
@@ -1284,10 +1286,10 @@
       <c r="D21" s="9">
         <v>255</v>
       </c>
-      <c r="E21" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="22"/>
+      <c r="E21" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="16"/>
       <c r="G21" s="4" t="s">
         <v>79</v>
       </c>
@@ -1302,10 +1304,10 @@
       <c r="D22" s="9">
         <v>255</v>
       </c>
-      <c r="E22" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" s="22"/>
+      <c r="E22" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="16"/>
       <c r="G22" s="4" t="s">
         <v>77</v>
       </c>
@@ -1320,10 +1322,10 @@
       <c r="D23" s="9">
         <v>255</v>
       </c>
-      <c r="E23" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F23" s="22"/>
+      <c r="E23" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="16"/>
       <c r="G23" s="4" t="s">
         <v>78</v>
       </c>
@@ -1338,10 +1340,10 @@
       <c r="D24" s="9">
         <v>255</v>
       </c>
-      <c r="E24" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F24" s="22"/>
+      <c r="E24" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="16"/>
       <c r="G24" s="4" t="s">
         <v>79</v>
       </c>
@@ -1356,10 +1358,10 @@
       <c r="D25" s="9">
         <v>255</v>
       </c>
-      <c r="E25" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F25" s="22"/>
+      <c r="E25" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="16"/>
       <c r="G25" s="4" t="s">
         <v>77</v>
       </c>
@@ -1374,10 +1376,10 @@
       <c r="D26" s="9">
         <v>255</v>
       </c>
-      <c r="E26" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" s="22"/>
+      <c r="E26" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="16"/>
       <c r="G26" s="4" t="s">
         <v>78</v>
       </c>
@@ -1392,10 +1394,10 @@
       <c r="D27" s="9">
         <v>255</v>
       </c>
-      <c r="E27" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="22"/>
+      <c r="E27" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="16"/>
       <c r="G27" s="4" t="s">
         <v>79</v>
       </c>
@@ -1410,10 +1412,10 @@
       <c r="D28" s="9">
         <v>255</v>
       </c>
-      <c r="E28" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="22"/>
+      <c r="E28" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="16"/>
       <c r="G28" s="4" t="s">
         <v>77</v>
       </c>
@@ -1428,10 +1430,10 @@
       <c r="D29" s="9">
         <v>255</v>
       </c>
-      <c r="E29" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="22"/>
+      <c r="E29" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="16"/>
       <c r="G29" s="4" t="s">
         <v>78</v>
       </c>
@@ -1446,10 +1448,10 @@
       <c r="D30" s="9">
         <v>255</v>
       </c>
-      <c r="E30" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="22"/>
+      <c r="E30" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="16"/>
       <c r="G30" s="4" t="s">
         <v>79</v>
       </c>
@@ -1464,10 +1466,10 @@
       <c r="D31" s="9">
         <v>255</v>
       </c>
-      <c r="E31" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F31" s="22"/>
+      <c r="E31" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="16"/>
       <c r="G31" s="4" t="s">
         <v>77</v>
       </c>
@@ -1482,10 +1484,10 @@
       <c r="D32" s="9">
         <v>255</v>
       </c>
-      <c r="E32" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F32" s="22"/>
+      <c r="E32" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="16"/>
       <c r="G32" s="4" t="s">
         <v>78</v>
       </c>
@@ -1500,10 +1502,10 @@
       <c r="D33" s="9">
         <v>255</v>
       </c>
-      <c r="E33" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F33" s="22"/>
+      <c r="E33" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="16"/>
       <c r="G33" s="4" t="s">
         <v>79</v>
       </c>
@@ -1518,10 +1520,10 @@
       <c r="D34" s="9">
         <v>255</v>
       </c>
-      <c r="E34" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34" s="22"/>
+      <c r="E34" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="16"/>
       <c r="G34" s="4" t="s">
         <v>77</v>
       </c>
@@ -1536,10 +1538,10 @@
       <c r="D35" s="9">
         <v>255</v>
       </c>
-      <c r="E35" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="22"/>
+      <c r="E35" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="16"/>
       <c r="G35" s="4" t="s">
         <v>78</v>
       </c>
@@ -1554,10 +1556,10 @@
       <c r="D36" s="9">
         <v>255</v>
       </c>
-      <c r="E36" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F36" s="22"/>
+      <c r="E36" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="16"/>
       <c r="G36" s="4" t="s">
         <v>79</v>
       </c>
@@ -1572,10 +1574,10 @@
       <c r="D37" s="9">
         <v>255</v>
       </c>
-      <c r="E37" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="22"/>
+      <c r="E37" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="16"/>
       <c r="G37" s="4" t="s">
         <v>77</v>
       </c>
@@ -1590,10 +1592,10 @@
       <c r="D38" s="9">
         <v>255</v>
       </c>
-      <c r="E38" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="22"/>
+      <c r="E38" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="16"/>
       <c r="G38" s="4" t="s">
         <v>78</v>
       </c>
@@ -1608,10 +1610,10 @@
       <c r="D39" s="9">
         <v>255</v>
       </c>
-      <c r="E39" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="22"/>
+      <c r="E39" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="16"/>
       <c r="G39" s="4" t="s">
         <v>79</v>
       </c>
@@ -1626,10 +1628,10 @@
       <c r="D40" s="9">
         <v>255</v>
       </c>
-      <c r="E40" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F40" s="22"/>
+      <c r="E40" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="16"/>
       <c r="G40" s="4" t="s">
         <v>77</v>
       </c>
@@ -1644,10 +1646,10 @@
       <c r="D41" s="9">
         <v>255</v>
       </c>
-      <c r="E41" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="22"/>
+      <c r="E41" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="16"/>
       <c r="G41" s="4" t="s">
         <v>78</v>
       </c>
@@ -1662,10 +1664,10 @@
       <c r="D42" s="9">
         <v>255</v>
       </c>
-      <c r="E42" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="22"/>
+      <c r="E42" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="16"/>
       <c r="G42" s="4" t="s">
         <v>79</v>
       </c>
@@ -1680,10 +1682,10 @@
       <c r="D43" s="9">
         <v>255</v>
       </c>
-      <c r="E43" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" s="22"/>
+      <c r="E43" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="16"/>
       <c r="G43" s="4" t="s">
         <v>77</v>
       </c>
@@ -1698,10 +1700,10 @@
       <c r="D44" s="9">
         <v>255</v>
       </c>
-      <c r="E44" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F44" s="22"/>
+      <c r="E44" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" s="16"/>
       <c r="G44" s="4" t="s">
         <v>78</v>
       </c>
@@ -1716,10 +1718,10 @@
       <c r="D45" s="9">
         <v>255</v>
       </c>
-      <c r="E45" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F45" s="22"/>
+      <c r="E45" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" s="16"/>
       <c r="G45" s="4" t="s">
         <v>79</v>
       </c>
@@ -1734,10 +1736,10 @@
       <c r="D46" s="9">
         <v>255</v>
       </c>
-      <c r="E46" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F46" s="22"/>
+      <c r="E46" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F46" s="16"/>
       <c r="G46" s="4" t="s">
         <v>77</v>
       </c>
@@ -1752,10 +1754,10 @@
       <c r="D47" s="9">
         <v>255</v>
       </c>
-      <c r="E47" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F47" s="22"/>
+      <c r="E47" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" s="16"/>
       <c r="G47" s="4" t="s">
         <v>78</v>
       </c>
@@ -1770,10 +1772,10 @@
       <c r="D48" s="9">
         <v>255</v>
       </c>
-      <c r="E48" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F48" s="22"/>
+      <c r="E48" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F48" s="16"/>
       <c r="G48" s="4" t="s">
         <v>79</v>
       </c>
@@ -1788,10 +1790,10 @@
       <c r="D49" s="9">
         <v>255</v>
       </c>
-      <c r="E49" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F49" s="22"/>
+      <c r="E49" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" s="16"/>
       <c r="G49" s="4" t="s">
         <v>77</v>
       </c>
@@ -1806,10 +1808,10 @@
       <c r="D50" s="9">
         <v>255</v>
       </c>
-      <c r="E50" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F50" s="22"/>
+      <c r="E50" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" s="16"/>
       <c r="G50" s="4" t="s">
         <v>78</v>
       </c>
@@ -1824,10 +1826,10 @@
       <c r="D51" s="9">
         <v>255</v>
       </c>
-      <c r="E51" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F51" s="22"/>
+      <c r="E51" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F51" s="16"/>
       <c r="G51" s="4" t="s">
         <v>79</v>
       </c>
@@ -1842,10 +1844,10 @@
       <c r="D52" s="9">
         <v>255</v>
       </c>
-      <c r="E52" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F52" s="22"/>
+      <c r="E52" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="16"/>
       <c r="G52" s="4" t="s">
         <v>77</v>
       </c>
@@ -1860,10 +1862,10 @@
       <c r="D53" s="9">
         <v>255</v>
       </c>
-      <c r="E53" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F53" s="22"/>
+      <c r="E53" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F53" s="16"/>
       <c r="G53" s="4" t="s">
         <v>78</v>
       </c>
@@ -1878,10 +1880,10 @@
       <c r="D54" s="9">
         <v>255</v>
       </c>
-      <c r="E54" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F54" s="22"/>
+      <c r="E54" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F54" s="16"/>
       <c r="G54" s="4" t="s">
         <v>79</v>
       </c>
@@ -1896,10 +1898,10 @@
       <c r="D55" s="9">
         <v>255</v>
       </c>
-      <c r="E55" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F55" s="22"/>
+      <c r="E55" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F55" s="16"/>
       <c r="G55" s="4" t="s">
         <v>77</v>
       </c>
@@ -1914,10 +1916,10 @@
       <c r="D56" s="9">
         <v>255</v>
       </c>
-      <c r="E56" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F56" s="22"/>
+      <c r="E56" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F56" s="16"/>
       <c r="G56" s="4" t="s">
         <v>78</v>
       </c>
@@ -1932,10 +1934,10 @@
       <c r="D57" s="9">
         <v>255</v>
       </c>
-      <c r="E57" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F57" s="22"/>
+      <c r="E57" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F57" s="16"/>
       <c r="G57" s="4" t="s">
         <v>79</v>
       </c>
@@ -1950,10 +1952,10 @@
       <c r="D58" s="9">
         <v>255</v>
       </c>
-      <c r="E58" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F58" s="22"/>
+      <c r="E58" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F58" s="16"/>
       <c r="G58" s="4" t="s">
         <v>77</v>
       </c>
@@ -1968,10 +1970,10 @@
       <c r="D59" s="9">
         <v>255</v>
       </c>
-      <c r="E59" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F59" s="22"/>
+      <c r="E59" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F59" s="16"/>
       <c r="G59" s="4" t="s">
         <v>78</v>
       </c>
@@ -1986,10 +1988,10 @@
       <c r="D60" s="9">
         <v>255</v>
       </c>
-      <c r="E60" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F60" s="22"/>
+      <c r="E60" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F60" s="16"/>
       <c r="G60" s="4" t="s">
         <v>79</v>
       </c>
@@ -2004,10 +2006,10 @@
       <c r="D61" s="9">
         <v>255</v>
       </c>
-      <c r="E61" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F61" s="22"/>
+      <c r="E61" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F61" s="16"/>
       <c r="G61" s="4" t="s">
         <v>77</v>
       </c>
@@ -2022,10 +2024,10 @@
       <c r="D62" s="9">
         <v>255</v>
       </c>
-      <c r="E62" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F62" s="22"/>
+      <c r="E62" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F62" s="16"/>
       <c r="G62" s="4" t="s">
         <v>78</v>
       </c>
@@ -2040,10 +2042,10 @@
       <c r="D63" s="9">
         <v>255</v>
       </c>
-      <c r="E63" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F63" s="22"/>
+      <c r="E63" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F63" s="16"/>
       <c r="G63" s="4" t="s">
         <v>79</v>
       </c>
@@ -2058,10 +2060,10 @@
       <c r="D64" s="9">
         <v>255</v>
       </c>
-      <c r="E64" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F64" s="22"/>
+      <c r="E64" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F64" s="16"/>
       <c r="G64" s="4" t="s">
         <v>77</v>
       </c>
@@ -2076,10 +2078,10 @@
       <c r="D65" s="9">
         <v>255</v>
       </c>
-      <c r="E65" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F65" s="22"/>
+      <c r="E65" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F65" s="16"/>
       <c r="G65" s="4" t="s">
         <v>78</v>
       </c>
@@ -2094,16 +2096,64 @@
       <c r="D66" s="9">
         <v>255</v>
       </c>
-      <c r="E66" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F66" s="22"/>
+      <c r="E66" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F66" s="16"/>
       <c r="G66" s="4" t="s">
         <v>79</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="64">
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E50:F50"/>
     <mergeCell ref="E64:F64"/>
     <mergeCell ref="E65:F65"/>
     <mergeCell ref="E66:F66"/>
@@ -2120,54 +2170,6 @@
     <mergeCell ref="E55:F55"/>
     <mergeCell ref="E56:F56"/>
     <mergeCell ref="E57:F57"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2176,6 +2178,493 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1F20BA3-F325-4AED-AFBF-798E8EDE0B26}">
+  <dimension ref="A1:C64"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="33">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <f>(A5-4)/3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="33"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="33"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="33">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <f>(A8-4)/3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="33"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="33"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="33">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <f>(A11-4)/3</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="33"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="33"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <f>(A14-4)/3</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <f>(A17-4)/3</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <f>(A20-4)/3</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>7</v>
+      </c>
+      <c r="C23">
+        <f>(A23-4)/3</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <f>(A26-4)/3</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>9</v>
+      </c>
+      <c r="C29">
+        <f>(A29-4)/3</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>10</v>
+      </c>
+      <c r="C32">
+        <f>(A32-4)/3</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="33">
+        <v>1</v>
+      </c>
+      <c r="C35">
+        <f>(A35-4)/3</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" s="33"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" s="33"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" s="33">
+        <v>2</v>
+      </c>
+      <c r="C38">
+        <f>(A38-4)/3</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" s="33"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" s="33"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" s="33">
+        <v>3</v>
+      </c>
+      <c r="C41">
+        <f>(A41-4)/3</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" s="33"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" s="33"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>4</v>
+      </c>
+      <c r="C44">
+        <f>(A44-4)/3</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>5</v>
+      </c>
+      <c r="C47">
+        <f>(A47-4)/3</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>6</v>
+      </c>
+      <c r="C50">
+        <f>(A50-4)/3</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>7</v>
+      </c>
+      <c r="C53">
+        <f>(A53-4)/3</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>8</v>
+      </c>
+      <c r="C56">
+        <f>(A56-4)/3</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>9</v>
+      </c>
+      <c r="C59">
+        <f>(A59-4)/3</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>10</v>
+      </c>
+      <c r="C62">
+        <f>(A62-4)/3</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFD3F556-A633-4208-B96C-79ABEEC1BD24}">
   <dimension ref="B2:H66"/>
   <sheetViews>
@@ -2203,11 +2692,11 @@
       <c r="D2" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="23"/>
-      <c r="G2" s="14" t="s">
+      <c r="F2" s="30"/>
+      <c r="G2" s="13" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2221,10 +2710,10 @@
       <c r="D3" s="6">
         <v>28</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="27">
         <v>28</v>
       </c>
-      <c r="F3" s="16"/>
+      <c r="F3" s="27"/>
       <c r="G3" s="4" t="s">
         <v>81</v>
       </c>
@@ -2239,10 +2728,10 @@
       <c r="D4" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="F4" s="19"/>
+      <c r="F4" s="31"/>
       <c r="G4" s="4" t="s">
         <v>82</v>
       </c>
@@ -2278,10 +2767,10 @@
       <c r="D6" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="F6" s="17"/>
+      <c r="F6" s="28"/>
       <c r="G6" s="4" t="s">
         <v>74</v>
       </c>
@@ -2297,10 +2786,10 @@
       <c r="D7" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" s="22"/>
+      <c r="E7" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="16"/>
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -2313,10 +2802,10 @@
       <c r="D8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="22"/>
+      <c r="E8" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="16"/>
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
@@ -2329,10 +2818,10 @@
       <c r="D9" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E9" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="22"/>
+      <c r="E9" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="16"/>
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -2345,10 +2834,10 @@
       <c r="D10" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F10" s="22"/>
+      <c r="E10" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="16"/>
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -2358,13 +2847,13 @@
       <c r="C11" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="F11" s="19"/>
+      <c r="F11" s="31"/>
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
@@ -2377,10 +2866,10 @@
       <c r="D12" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12" s="22"/>
+      <c r="E12" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="16"/>
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
@@ -2393,10 +2882,10 @@
       <c r="D13" s="9">
         <v>255</v>
       </c>
-      <c r="E13" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="22"/>
+      <c r="E13" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="16"/>
       <c r="G13" s="4" t="s">
         <v>77</v>
       </c>
@@ -2411,10 +2900,10 @@
       <c r="D14" s="9">
         <v>255</v>
       </c>
-      <c r="E14" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" s="22"/>
+      <c r="E14" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="16"/>
       <c r="G14" s="4" t="s">
         <v>78</v>
       </c>
@@ -2429,10 +2918,10 @@
       <c r="D15" s="9">
         <v>255</v>
       </c>
-      <c r="E15" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="22"/>
+      <c r="E15" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="16"/>
       <c r="G15" s="4" t="s">
         <v>79</v>
       </c>
@@ -2447,10 +2936,10 @@
       <c r="D16" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E16" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F16" s="22"/>
+      <c r="E16" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" s="16"/>
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
@@ -2463,10 +2952,10 @@
       <c r="D17" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E17" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F17" s="22"/>
+      <c r="E17" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="16"/>
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
@@ -2479,10 +2968,10 @@
       <c r="D18" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E18" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F18" s="22"/>
+      <c r="E18" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" s="16"/>
       <c r="G18" s="4"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
@@ -2495,10 +2984,10 @@
       <c r="D19" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E19" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F19" s="22"/>
+      <c r="E19" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="16"/>
       <c r="G19" s="4"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
@@ -2511,10 +3000,10 @@
       <c r="D20" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E20" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F20" s="22"/>
+      <c r="E20" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" s="16"/>
       <c r="G20" s="4"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
@@ -2527,10 +3016,10 @@
       <c r="D21" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E21" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F21" s="22"/>
+      <c r="E21" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" s="16"/>
       <c r="G21" s="4"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
@@ -2543,10 +3032,10 @@
       <c r="D22" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E22" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F22" s="22"/>
+      <c r="E22" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="16"/>
       <c r="G22" s="4"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
@@ -2559,10 +3048,10 @@
       <c r="D23" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E23" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F23" s="22"/>
+      <c r="E23" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F23" s="16"/>
       <c r="G23" s="4"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
@@ -2575,10 +3064,10 @@
       <c r="D24" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E24" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F24" s="22"/>
+      <c r="E24" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F24" s="16"/>
       <c r="G24" s="4"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
@@ -2591,10 +3080,10 @@
       <c r="D25" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E25" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F25" s="22"/>
+      <c r="E25" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" s="16"/>
       <c r="G25" s="4"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
@@ -2607,10 +3096,10 @@
       <c r="D26" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E26" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F26" s="22"/>
+      <c r="E26" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" s="16"/>
       <c r="G26" s="4"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
@@ -2623,10 +3112,10 @@
       <c r="D27" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E27" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F27" s="22"/>
+      <c r="E27" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" s="16"/>
       <c r="G27" s="4"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
@@ -2639,10 +3128,10 @@
       <c r="D28" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E28" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F28" s="22"/>
+      <c r="E28" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F28" s="16"/>
       <c r="G28" s="4"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
@@ -2655,10 +3144,10 @@
       <c r="D29" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E29" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F29" s="22"/>
+      <c r="E29" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" s="16"/>
       <c r="G29" s="4"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
@@ -2671,10 +3160,10 @@
       <c r="D30" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E30" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F30" s="22"/>
+      <c r="E30" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F30" s="16"/>
       <c r="G30" s="4"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
@@ -2687,10 +3176,10 @@
       <c r="D31" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E31" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F31" s="22"/>
+      <c r="E31" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F31" s="16"/>
       <c r="G31" s="4"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
@@ -2703,10 +3192,10 @@
       <c r="D32" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E32" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F32" s="22"/>
+      <c r="E32" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F32" s="16"/>
       <c r="G32" s="4"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.25">
@@ -2719,10 +3208,10 @@
       <c r="D33" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E33" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F33" s="22"/>
+      <c r="E33" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F33" s="16"/>
       <c r="G33" s="4"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
@@ -2735,10 +3224,10 @@
       <c r="D34" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E34" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F34" s="22"/>
+      <c r="E34" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F34" s="16"/>
       <c r="G34" s="4"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.25">
@@ -2751,10 +3240,10 @@
       <c r="D35" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E35" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F35" s="22"/>
+      <c r="E35" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F35" s="16"/>
       <c r="G35" s="4"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
@@ -2767,10 +3256,10 @@
       <c r="D36" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E36" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F36" s="22"/>
+      <c r="E36" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F36" s="16"/>
       <c r="G36" s="4"/>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
@@ -2783,10 +3272,10 @@
       <c r="D37" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E37" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F37" s="22"/>
+      <c r="E37" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F37" s="16"/>
       <c r="G37" s="4"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
@@ -2799,10 +3288,10 @@
       <c r="D38" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E38" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F38" s="22"/>
+      <c r="E38" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F38" s="16"/>
       <c r="G38" s="4"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
@@ -2815,10 +3304,10 @@
       <c r="D39" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E39" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F39" s="22"/>
+      <c r="E39" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F39" s="16"/>
       <c r="G39" s="4"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
@@ -2831,10 +3320,10 @@
       <c r="D40" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E40" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F40" s="22"/>
+      <c r="E40" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F40" s="16"/>
       <c r="G40" s="4"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
@@ -2847,10 +3336,10 @@
       <c r="D41" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E41" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F41" s="22"/>
+      <c r="E41" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F41" s="16"/>
       <c r="G41" s="4"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.25">
@@ -2863,10 +3352,10 @@
       <c r="D42" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E42" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F42" s="22"/>
+      <c r="E42" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F42" s="16"/>
       <c r="G42" s="4"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.25">
@@ -2879,10 +3368,10 @@
       <c r="D43" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E43" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F43" s="22"/>
+      <c r="E43" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F43" s="16"/>
       <c r="G43" s="4"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.25">
@@ -2895,10 +3384,10 @@
       <c r="D44" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E44" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F44" s="22"/>
+      <c r="E44" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F44" s="16"/>
       <c r="G44" s="4"/>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.25">
@@ -2911,10 +3400,10 @@
       <c r="D45" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E45" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F45" s="22"/>
+      <c r="E45" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F45" s="16"/>
       <c r="G45" s="4"/>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.25">
@@ -2927,10 +3416,10 @@
       <c r="D46" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E46" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F46" s="22"/>
+      <c r="E46" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F46" s="16"/>
       <c r="G46" s="4"/>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.25">
@@ -2943,10 +3432,10 @@
       <c r="D47" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E47" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F47" s="22"/>
+      <c r="E47" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F47" s="16"/>
       <c r="G47" s="4"/>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.25">
@@ -2959,10 +3448,10 @@
       <c r="D48" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E48" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F48" s="22"/>
+      <c r="E48" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F48" s="16"/>
       <c r="G48" s="4"/>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.25">
@@ -2975,10 +3464,10 @@
       <c r="D49" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E49" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F49" s="22"/>
+      <c r="E49" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F49" s="16"/>
       <c r="G49" s="4"/>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.25">
@@ -2991,10 +3480,10 @@
       <c r="D50" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E50" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F50" s="22"/>
+      <c r="E50" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F50" s="16"/>
       <c r="G50" s="4"/>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.25">
@@ -3007,10 +3496,10 @@
       <c r="D51" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E51" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F51" s="22"/>
+      <c r="E51" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F51" s="16"/>
       <c r="G51" s="4"/>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.25">
@@ -3023,10 +3512,10 @@
       <c r="D52" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E52" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F52" s="22"/>
+      <c r="E52" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F52" s="16"/>
       <c r="G52" s="4"/>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.25">
@@ -3039,10 +3528,10 @@
       <c r="D53" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E53" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F53" s="22"/>
+      <c r="E53" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F53" s="16"/>
       <c r="G53" s="4"/>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.25">
@@ -3055,10 +3544,10 @@
       <c r="D54" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E54" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F54" s="22"/>
+      <c r="E54" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F54" s="16"/>
       <c r="G54" s="4"/>
     </row>
     <row r="55" spans="2:7" x14ac:dyDescent="0.25">
@@ -3071,10 +3560,10 @@
       <c r="D55" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E55" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F55" s="22"/>
+      <c r="E55" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F55" s="16"/>
       <c r="G55" s="4"/>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.25">
@@ -3087,10 +3576,10 @@
       <c r="D56" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E56" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F56" s="22"/>
+      <c r="E56" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F56" s="16"/>
       <c r="G56" s="4"/>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.25">
@@ -3103,10 +3592,10 @@
       <c r="D57" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E57" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F57" s="22"/>
+      <c r="E57" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F57" s="16"/>
       <c r="G57" s="4"/>
     </row>
     <row r="58" spans="2:7" x14ac:dyDescent="0.25">
@@ -3119,10 +3608,10 @@
       <c r="D58" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E58" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F58" s="22"/>
+      <c r="E58" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F58" s="16"/>
       <c r="G58" s="4"/>
     </row>
     <row r="59" spans="2:7" x14ac:dyDescent="0.25">
@@ -3135,10 +3624,10 @@
       <c r="D59" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E59" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F59" s="22"/>
+      <c r="E59" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F59" s="16"/>
       <c r="G59" s="4"/>
     </row>
     <row r="60" spans="2:7" x14ac:dyDescent="0.25">
@@ -3151,10 +3640,10 @@
       <c r="D60" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E60" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F60" s="22"/>
+      <c r="E60" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F60" s="16"/>
       <c r="G60" s="4"/>
     </row>
     <row r="61" spans="2:7" x14ac:dyDescent="0.25">
@@ -3167,10 +3656,10 @@
       <c r="D61" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E61" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F61" s="22"/>
+      <c r="E61" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F61" s="16"/>
       <c r="G61" s="4"/>
     </row>
     <row r="62" spans="2:7" x14ac:dyDescent="0.25">
@@ -3183,10 +3672,10 @@
       <c r="D62" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E62" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F62" s="22"/>
+      <c r="E62" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F62" s="16"/>
       <c r="G62" s="4"/>
     </row>
     <row r="63" spans="2:7" x14ac:dyDescent="0.25">
@@ -3199,10 +3688,10 @@
       <c r="D63" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E63" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F63" s="22"/>
+      <c r="E63" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F63" s="16"/>
       <c r="G63" s="4"/>
     </row>
     <row r="64" spans="2:7" x14ac:dyDescent="0.25">
@@ -3215,10 +3704,10 @@
       <c r="D64" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E64" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F64" s="22"/>
+      <c r="E64" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F64" s="16"/>
       <c r="G64" s="4"/>
     </row>
     <row r="65" spans="2:7" x14ac:dyDescent="0.25">
@@ -3231,10 +3720,10 @@
       <c r="D65" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E65" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F65" s="22"/>
+      <c r="E65" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F65" s="16"/>
       <c r="G65" s="4"/>
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.25">
@@ -3247,14 +3736,70 @@
       <c r="D66" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E66" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F66" s="22"/>
+      <c r="E66" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F66" s="16"/>
       <c r="G66" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="64">
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="E57:F57"/>
     <mergeCell ref="E65:F65"/>
     <mergeCell ref="E66:F66"/>
     <mergeCell ref="E59:F59"/>
@@ -3263,62 +3808,6 @@
     <mergeCell ref="E62:F62"/>
     <mergeCell ref="E63:F63"/>
     <mergeCell ref="E64:F64"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>